<commit_message>
Changed categories to hints
</commit_message>
<xml_diff>
--- a/Assets/Questions/Questions.xlsx
+++ b/Assets/Questions/Questions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Question</t>
   </si>
@@ -50,9 +50,6 @@
     <t>52 Weeks IN A Year</t>
   </si>
   <si>
-    <t>Elementary School</t>
-  </si>
-  <si>
     <t>44 Countries IN Europe</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>10 Provinces IN Canada</t>
   </si>
   <si>
-    <t>4 Countries IN THE United Kingdom</t>
-  </si>
-  <si>
     <t>5 Oceans IN THE World</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>8 Movies IN Harry Potter</t>
   </si>
   <si>
-    <t>7 Books IN THE Chronicles Of Narnia</t>
-  </si>
-  <si>
     <t>86400 Seconds IN A Day</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>16 Tablespoons IN A Cup</t>
   </si>
   <si>
-    <t>Food</t>
-  </si>
-  <si>
     <t>24 Timezones IN THE World</t>
   </si>
   <si>
@@ -113,12 +101,6 @@
     <t>40 Quarters IN A Roll</t>
   </si>
   <si>
-    <t>Random</t>
-  </si>
-  <si>
-    <t>118 Elements ON THE Periodic Table</t>
-  </si>
-  <si>
     <t>10 Years IN A Decade</t>
   </si>
   <si>
@@ -132,6 +114,39 @@
   </si>
   <si>
     <t>Hint</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Great Outdoors</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>Poetry</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Weather</t>
   </si>
 </sst>
 </file>
@@ -229,8 +244,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:B1048576">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B1048573" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:B1048573">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
@@ -539,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,55 +627,55 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,23 +683,23 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +707,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,31 +715,31 @@
         <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +747,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,47 +755,23 @@
         <v>26</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed problem with Baker's Dozen
</commit_message>
<xml_diff>
--- a/Assets/Questions/Questions.xlsx
+++ b/Assets/Questions/Questions.xlsx
@@ -35,9 +35,6 @@
     <t>365 Days IN A Year</t>
   </si>
   <si>
-    <t>13 Items IN A Baker's Dozen</t>
-  </si>
-  <si>
     <t>8 Planets IN THE Milky Way</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>21 Points IN Badminton</t>
+  </si>
+  <si>
+    <t>13 Items IN A Bakers Dozen</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
   <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,255 +668,255 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -924,63 +924,63 @@
         <v>2</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -988,135 +988,135 @@
         <v>1</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed opening screen and removed suggest puzzle
</commit_message>
<xml_diff>
--- a/Assets/Questions/Questions.xlsx
+++ b/Assets/Questions/Questions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
   <si>
     <t>Question</t>
   </si>
@@ -240,6 +240,45 @@
   </si>
   <si>
     <t>13 Items IN A Bakers Dozen</t>
+  </si>
+  <si>
+    <t>6909 Languages IN THE World</t>
+  </si>
+  <si>
+    <t>3 Periods IN A Hockey Game</t>
+  </si>
+  <si>
+    <t>4 Quarters IN A Basketball Game</t>
+  </si>
+  <si>
+    <t>4 Periods IN A Lacrosse Game</t>
+  </si>
+  <si>
+    <t>5 Positions IN Basketball</t>
+  </si>
+  <si>
+    <t>4840 Square Yards IN A Acre</t>
+  </si>
+  <si>
+    <t>10000 Square Meters IN A Hectare</t>
+  </si>
+  <si>
+    <t>4 Grand Slams IN Tennis</t>
+  </si>
+  <si>
+    <t>8 Stones IN Curling</t>
+  </si>
+  <si>
+    <t>15 Sports IN THE Winter Olympics</t>
+  </si>
+  <si>
+    <t>28 Sports IN THE Summer Olympics</t>
+  </si>
+  <si>
+    <t>23 Cities HOSTED Summer Olympics</t>
+  </si>
+  <si>
+    <t>16 Cities HOSTED Winter Olympics</t>
   </si>
 </sst>
 </file>
@@ -337,8 +376,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B1048568" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:B1048568">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B1048567" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:B1048567">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
@@ -650,11 +689,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,6 +1158,110 @@
         <v>18</v>
       </c>
     </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New questions and reordered questions
</commit_message>
<xml_diff>
--- a/Assets/Questions/Questions.xlsx
+++ b/Assets/Questions/Questions.xlsx
@@ -213,9 +213,6 @@
     <t>5 Vowels IN THE English Alphabet</t>
   </si>
   <si>
-    <t>26 Letters IN THE English Alphabet</t>
-  </si>
-  <si>
     <t>58 Breeds OF Cat</t>
   </si>
   <si>
@@ -547,6 +544,9 @@
   </si>
   <si>
     <t>6852 Islands IN Japan</t>
+  </si>
+  <si>
+    <t>26 Letters IN THE Alphabet</t>
   </si>
 </sst>
 </file>
@@ -649,9 +649,6 @@
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
-  <sortState ref="A2:B151">
-    <sortCondition ref="B1"/>
-  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" name="Question" dataDxfId="1"/>
     <tableColumn id="2" name="Hint" dataDxfId="0"/>
@@ -960,8 +957,8 @@
   <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B151" sqref="A1:B151"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,247 +977,247 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>169</v>
+        <v>85</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>10</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>10</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>14</v>
+        <v>145</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>10</v>
@@ -1228,39 +1225,39 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>10</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>10</v>
@@ -1268,47 +1265,47 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>10</v>
@@ -1316,279 +1313,279 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>149</v>
+        <v>66</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>166</v>
+        <v>59</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>173</v>
+        <v>77</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>142</v>
+        <v>75</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>138</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>36</v>
+        <v>156</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>25</v>
@@ -1596,15 +1593,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>25</v>
@@ -1612,7 +1609,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>25</v>
@@ -1620,15 +1617,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>25</v>
@@ -1636,546 +1633,546 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>152</v>
+        <v>13</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>3</v>
+        <v>147</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>125</v>
+        <v>57</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>127</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>28</v>
+        <v>126</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>